<commit_message>
Domino Di Rev. A: added slider switch
</commit_message>
<xml_diff>
--- a/Domino Di/BOM/Domino Di BOM.xlsx
+++ b/Domino Di/BOM/Domino Di BOM.xlsx
@@ -11,30 +11,31 @@
     <sheet name="Domino Di Rev. A" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Di Rev. A'!$A$3:$I$36</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Di Rev. A'!$A$3:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$3:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Di Rev. A'!$A$3:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$3:$I$36</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$34</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Di Rev. A'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
   <si>
     <t>Item</t>
   </si>
@@ -279,7 +280,7 @@
     <t>R0402_1k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R10</t>
+    <t>R11</t>
   </si>
   <si>
     <t>RES 1K OHM 1/16W 5% 0402 SMD</t>
@@ -294,7 +295,7 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R2, R5</t>
+    <t>R2, R4, R6</t>
   </si>
   <si>
     <t>RES 0.0 OHM 1/8W JUMP SMD 0603</t>
@@ -318,7 +319,7 @@
     <t>R0402_270R_5%_62.5mW</t>
   </si>
   <si>
-    <t>R4</t>
+    <t>R5</t>
   </si>
   <si>
     <t>RES 270 OHM 1/16W 5% 0402 SMD</t>
@@ -327,7 +328,7 @@
     <t>R0603_270R_5%_125mW</t>
   </si>
   <si>
-    <t>R6</t>
+    <t>R7</t>
   </si>
   <si>
     <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
@@ -336,7 +337,7 @@
     <t>R0402_0R_5%_62.5mW</t>
   </si>
   <si>
-    <t>R7, R9</t>
+    <t>R8, R10</t>
   </si>
   <si>
     <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
@@ -348,7 +349,7 @@
     <t>R0402_10k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R8</t>
+    <t>R9</t>
   </si>
   <si>
     <t>RES 10K OHM 1/16W 5% 0402 SMD</t>
@@ -372,10 +373,19 @@
     <t>CONN USB MICRO B RECPT SMT R/A</t>
   </si>
   <si>
+    <t>MK-12C01</t>
+  </si>
+  <si>
+    <t>SW1(DNP)</t>
+  </si>
+  <si>
+    <t>SLIDE SWITCH 1P2T 6V DC 0.3A</t>
+  </si>
+  <si>
     <t>IT-1210</t>
   </si>
   <si>
-    <t>SW1</t>
+    <t>SW2</t>
   </si>
   <si>
     <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
@@ -526,7 +536,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -572,505 +582,502 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -1082,198 +1089,198 @@
         <v>10</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>107</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>107</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>